<commit_message>
false positives, code refactor, plot
</commit_message>
<xml_diff>
--- a/false_positives/summary_df.xlsx
+++ b/false_positives/summary_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,89 +453,89 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>tls_root_cert_validity_len</t>
+          <t>rdap_domain_age</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1349</v>
+        <v>9.04408292e+17</v>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1135</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C3" t="n">
-        <v>79</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>dns_soa_retry</t>
+          <t>rdap_time_from_last_change</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>900</v>
+        <v>4.00056294e+17</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ip_v4_count</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11</v>
+        <v>5078</v>
       </c>
       <c r="C5" t="n">
-        <v>19</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>dns_TXT_count</t>
+          <t>tls_root_cert_validity_len</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>1349</v>
       </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>dns_dn_level</t>
+          <t>rdap_ip_longest_v4_prefix_len</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>dns_resolved_record_types</t>
+          <t>lex_name_len</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C8" t="n">
         <v>1</v>
@@ -544,62 +544,118 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>ip_v4_count</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.53</v>
+        <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
+          <t>lex_tld_len</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
+          <t>dns_dn_level</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr"/>
+          <t>ip_as_address_entropy</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>2</v>
+      </c>
       <c r="C12" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
+          <t>lex_sub_digit_ratio</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.67</v>
+      </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>dns_zone_entropy</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="C14" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>dns_ttl_low</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>rdap_registrar_name_hash</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
virus total, fp check
</commit_message>
<xml_diff>
--- a/false_positives/summary_df.xlsx
+++ b/false_positives/summary_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D170"/>
+  <dimension ref="A1:D175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,72 +458,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.04408292e+17</v>
+        <v>8.931168e+17</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>bannerlord-service-discovery.bannerlord-services-2.net</t>
+          <t>yeeterracing.com</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>9.04408292e+17</v>
+        <v>8.931168e+17</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>yeeterracing.com</t>
+          <t>ticks2.bugsense.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>9.04408292e+17</v>
+        <v>8.931168e+17</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>video.browser.tvall.cn</t>
+          <t>www.zhcsm.cn</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>9.04408292e+17</v>
+        <v>8.931168e+17</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>gpvjyx.ssptp4.com</t>
+          <t>edoardocolombo.eu</t>
         </is>
       </c>
     </row>
@@ -534,14 +534,14 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.2576e+17</v>
+        <v>8.931168e+17</v>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>www.zhcsm.cn</t>
+          <t>synapse.caterpillarcheesecake.xyz</t>
         </is>
       </c>
     </row>
@@ -552,140 +552,140 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7.2576e+17</v>
+        <v>8.931168e+17</v>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>babbage.betadome.net</t>
+          <t>www.studiumarteterapie.cz</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>rdap_registrar_name_hash</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>7.2576e+17</v>
+        <v>1757849580</v>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>solnicka.sk</t>
+          <t>bihamcurchef.cam</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>7.2576e+17</v>
+        <v>5078</v>
       </c>
       <c r="C9" t="n">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>intouchservices.com</t>
+          <t>torrentsnows.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7.2576e+17</v>
+        <v>5078</v>
       </c>
       <c r="C10" t="n">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>edoardocolombo.eu</t>
+          <t>connect.proxytx.cloud</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7.2576e+17</v>
+        <v>5078</v>
       </c>
       <c r="C11" t="n">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>avt-usa.net</t>
+          <t>torrentz2.eu</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7.2576e+17</v>
+        <v>5078</v>
       </c>
       <c r="C12" t="n">
-        <v>7</v>
+        <v>86</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>www.studiumarteterapie.cz</t>
+          <t>sensagent.leparisien.fr</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>rdap_time_from_last_change</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4.00056294e+17</v>
+        <v>5078</v>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>torrentsmd.me</t>
+          <t>airportus.info</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>rdap_time_from_last_change</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>4.00056294e+17</v>
+        <v>5078</v>
       </c>
       <c r="C14" t="n">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>toubiz.de</t>
+          <t>time.alcanet.no</t>
         </is>
       </c>
     </row>
@@ -699,11 +699,11 @@
         <v>5078</v>
       </c>
       <c r="C15" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>sso.kkarau.edu.my</t>
+          <t>backupaccount.com</t>
         </is>
       </c>
     </row>
@@ -717,11 +717,11 @@
         <v>5078</v>
       </c>
       <c r="C16" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>smaxdn.com</t>
+          <t>pthikitpet.com</t>
         </is>
       </c>
     </row>
@@ -735,11 +735,11 @@
         <v>5078</v>
       </c>
       <c r="C17" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>doogh.club</t>
+          <t>one.exness.link</t>
         </is>
       </c>
     </row>
@@ -753,11 +753,11 @@
         <v>5078</v>
       </c>
       <c r="C18" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>torrentz2.eu</t>
+          <t>api.wmkankan.com</t>
         </is>
       </c>
     </row>
@@ -771,11 +771,11 @@
         <v>5078</v>
       </c>
       <c r="C19" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>blibli.gw-dv.net</t>
+          <t>awecerybtuitbyatr.com</t>
         </is>
       </c>
     </row>
@@ -789,11 +789,11 @@
         <v>5078</v>
       </c>
       <c r="C20" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>torrent-download.to</t>
+          <t>gm2.iinmobi.com</t>
         </is>
       </c>
     </row>
@@ -807,11 +807,11 @@
         <v>5078</v>
       </c>
       <c r="C21" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>games4.qqgametimes.com</t>
+          <t>airasia.gw-dv.net</t>
         </is>
       </c>
     </row>
@@ -825,11 +825,11 @@
         <v>5078</v>
       </c>
       <c r="C22" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>torrentsnows.com</t>
+          <t>stra.hasmobi.net</t>
         </is>
       </c>
     </row>
@@ -843,11 +843,11 @@
         <v>5078</v>
       </c>
       <c r="C23" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>intensive.int</t>
+          <t>s.ktxtr.com</t>
         </is>
       </c>
     </row>
@@ -861,11 +861,11 @@
         <v>5078</v>
       </c>
       <c r="C24" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>auth.merrillcorp.com</t>
+          <t>www.dontgobaconmyheart.co.uk</t>
         </is>
       </c>
     </row>
@@ -879,11 +879,11 @@
         <v>5078</v>
       </c>
       <c r="C25" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>chishir.com</t>
+          <t>www.estrenospapaya.com</t>
         </is>
       </c>
     </row>
@@ -897,11 +897,11 @@
         <v>5078</v>
       </c>
       <c r="C26" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>audiotel.com.mx</t>
+          <t>eservices.manpower.gov.om</t>
         </is>
       </c>
     </row>
@@ -915,11 +915,11 @@
         <v>5078</v>
       </c>
       <c r="C27" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>szhxws.com</t>
+          <t>www.laboratore-proti-koronaviru.cz</t>
         </is>
       </c>
     </row>
@@ -933,11 +933,11 @@
         <v>5078</v>
       </c>
       <c r="C28" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>airportus.info</t>
+          <t>smaxdn.com</t>
         </is>
       </c>
     </row>
@@ -951,11 +951,11 @@
         <v>5078</v>
       </c>
       <c r="C29" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>onlineworkplace24.de</t>
+          <t>doogh.club</t>
         </is>
       </c>
     </row>
@@ -969,11 +969,11 @@
         <v>5078</v>
       </c>
       <c r="C30" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>time.alcanet.no</t>
+          <t>blibli.gw-dv.net</t>
         </is>
       </c>
     </row>
@@ -987,11 +987,11 @@
         <v>5078</v>
       </c>
       <c r="C31" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>leavehomesafe.gov.hk</t>
+          <t>torrent-download.to</t>
         </is>
       </c>
     </row>
@@ -1005,11 +1005,11 @@
         <v>5078</v>
       </c>
       <c r="C32" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>r.blok.link</t>
+          <t>vid-play.com</t>
         </is>
       </c>
     </row>
@@ -1023,11 +1023,11 @@
         <v>5078</v>
       </c>
       <c r="C33" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>ppp.xxpwgxx.com</t>
+          <t>intensive.int</t>
         </is>
       </c>
     </row>
@@ -1041,11 +1041,11 @@
         <v>5078</v>
       </c>
       <c r="C34" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>api.video.browser.tvall.cn</t>
+          <t>chishir.com</t>
         </is>
       </c>
     </row>
@@ -1059,11 +1059,11 @@
         <v>5078</v>
       </c>
       <c r="C35" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>connect.dewvpn.cc</t>
+          <t>szhxws.com</t>
         </is>
       </c>
     </row>
@@ -1077,11 +1077,11 @@
         <v>5078</v>
       </c>
       <c r="C36" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>discordapp.page.link</t>
+          <t>duckduckmooseapps.com</t>
         </is>
       </c>
     </row>
@@ -1095,11 +1095,11 @@
         <v>5078</v>
       </c>
       <c r="C37" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>endpointdns-gcprod-use1-lb.jfrog.io</t>
+          <t>www.1ucn.com</t>
         </is>
       </c>
     </row>
@@ -1113,11 +1113,11 @@
         <v>5078</v>
       </c>
       <c r="C38" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>pthikitpet.com</t>
+          <t>leavehomesafe.gov.hk</t>
         </is>
       </c>
     </row>
@@ -1131,11 +1131,11 @@
         <v>5078</v>
       </c>
       <c r="C39" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>one.exness.link</t>
+          <t>r.blok.link</t>
         </is>
       </c>
     </row>
@@ -1149,11 +1149,11 @@
         <v>5078</v>
       </c>
       <c r="C40" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>www.centrumprenatalnidiagnostiky.cz</t>
+          <t>tvtelemetrie.de</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1167,11 @@
         <v>5078</v>
       </c>
       <c r="C41" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>vafrike.ru</t>
+          <t>connect.dewvpn.cc</t>
         </is>
       </c>
     </row>
@@ -1185,11 +1185,11 @@
         <v>5078</v>
       </c>
       <c r="C42" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>www.lnwpickpack.com</t>
+          <t>discordapp.page.link</t>
         </is>
       </c>
     </row>
@@ -1203,11 +1203,11 @@
         <v>5078</v>
       </c>
       <c r="C43" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>www.yandex.ua</t>
+          <t>rcmdodo.theirving.net</t>
         </is>
       </c>
     </row>
@@ -1221,11 +1221,11 @@
         <v>5078</v>
       </c>
       <c r="C44" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>api.wmkankan.com</t>
+          <t>www.centrumprenatalnidiagnostiky.cz</t>
         </is>
       </c>
     </row>
@@ -1239,11 +1239,11 @@
         <v>5078</v>
       </c>
       <c r="C45" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>awrcaverybrstuktdybstr.com</t>
+          <t>vafrike.ru</t>
         </is>
       </c>
     </row>
@@ -1257,11 +1257,11 @@
         <v>5078</v>
       </c>
       <c r="C46" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>awecerybtuitbyatr.com</t>
+          <t>ucmetrixa.info</t>
         </is>
       </c>
     </row>
@@ -1275,11 +1275,11 @@
         <v>5078</v>
       </c>
       <c r="C47" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>gm2.iinmobi.com</t>
+          <t>www.mz.de</t>
         </is>
       </c>
     </row>
@@ -1293,11 +1293,11 @@
         <v>5078</v>
       </c>
       <c r="C48" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>airasia.gw-dv.net</t>
+          <t>download.lenovoemc.com</t>
         </is>
       </c>
     </row>
@@ -1311,11 +1311,11 @@
         <v>5078</v>
       </c>
       <c r="C49" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>tcs-japan.co.jp</t>
+          <t>rtbonecode.com</t>
         </is>
       </c>
     </row>
@@ -1329,11 +1329,11 @@
         <v>5078</v>
       </c>
       <c r="C50" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>stra.hasmobi.net</t>
+          <t>time.nimatronicc.xyz</t>
         </is>
       </c>
     </row>
@@ -1347,11 +1347,11 @@
         <v>5078</v>
       </c>
       <c r="C51" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>speed-app.com</t>
+          <t>cdn.bitrix24.ua</t>
         </is>
       </c>
     </row>
@@ -1365,11 +1365,11 @@
         <v>5078</v>
       </c>
       <c r="C52" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>s.ktxtr.com</t>
+          <t>bankinformation.1c.ru</t>
         </is>
       </c>
     </row>
@@ -1383,11 +1383,11 @@
         <v>5078</v>
       </c>
       <c r="C53" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>download.lenovoemc.com</t>
+          <t>laocaifengxitong.cc</t>
         </is>
       </c>
     </row>
@@ -1401,11 +1401,11 @@
         <v>5078</v>
       </c>
       <c r="C54" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>rtbonecode.com</t>
+          <t>ffe390afd658c19dcbf707e0597b846d.de.whecloud.com</t>
         </is>
       </c>
     </row>
@@ -1419,11 +1419,11 @@
         <v>5078</v>
       </c>
       <c r="C55" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>insoc.cloud</t>
+          <t>update.chupdatebrowserhosting.com</t>
         </is>
       </c>
     </row>
@@ -1437,11 +1437,11 @@
         <v>5078</v>
       </c>
       <c r="C56" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>time.nimatronicc.xyz</t>
+          <t>ppp.xxpwgxx.com</t>
         </is>
       </c>
     </row>
@@ -1455,11 +1455,11 @@
         <v>5078</v>
       </c>
       <c r="C57" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>www.estrenospapaya.com</t>
+          <t>sso.manpower.gov.om</t>
         </is>
       </c>
     </row>
@@ -1473,11 +1473,11 @@
         <v>5078</v>
       </c>
       <c r="C58" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>eservices.manpower.gov.om</t>
+          <t>www.cumonprintedpics.com</t>
         </is>
       </c>
     </row>
@@ -1491,11 +1491,11 @@
         <v>5078</v>
       </c>
       <c r="C59" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>os-api.test.os.qkcorp.net</t>
+          <t>www.yandex.ua</t>
         </is>
       </c>
     </row>
@@ -1509,11 +1509,11 @@
         <v>5078</v>
       </c>
       <c r="C60" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>microgalon.com</t>
+          <t>vejasp.abril.com.br</t>
         </is>
       </c>
     </row>
@@ -1527,11 +1527,11 @@
         <v>5078</v>
       </c>
       <c r="C61" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>catpitaqmi.net</t>
+          <t>api.tinyhoneybee.com</t>
         </is>
       </c>
     </row>
@@ -1545,11 +1545,11 @@
         <v>5078</v>
       </c>
       <c r="C62" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>bankinformation.1c.ru</t>
+          <t>services.keepersecurity.eu</t>
         </is>
       </c>
     </row>
@@ -1563,11 +1563,11 @@
         <v>5078</v>
       </c>
       <c r="C63" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>laocaifengxitong.cc</t>
+          <t>www.shorturl.at</t>
         </is>
       </c>
     </row>
@@ -1581,11 +1581,11 @@
         <v>5078</v>
       </c>
       <c r="C64" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>24.winprizes524.digital</t>
+          <t>transversalnavigation.gamu.cz</t>
         </is>
       </c>
     </row>
@@ -1599,11 +1599,11 @@
         <v>5078</v>
       </c>
       <c r="C65" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>update.chupdatebrowserhosting.com</t>
+          <t>speed-app.com</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         <v>5078</v>
       </c>
       <c r="C66" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>takungpao.com.hk</t>
+          <t>mp3nhacvui.net</t>
         </is>
       </c>
     </row>
@@ -1635,11 +1635,11 @@
         <v>5078</v>
       </c>
       <c r="C67" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>makeawesomeapps.com</t>
+          <t>wifihotspot.hu</t>
         </is>
       </c>
     </row>
@@ -1653,11 +1653,11 @@
         <v>5078</v>
       </c>
       <c r="C68" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>st-fakesysupgrade.fakevivo.com.cn</t>
+          <t>epiccareeverywhere.addenbrookes.nhs.uk</t>
         </is>
       </c>
     </row>
@@ -1671,11 +1671,11 @@
         <v>5078</v>
       </c>
       <c r="C69" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>tag.contactatonce.co.uk</t>
+          <t>imagodd.com</t>
         </is>
       </c>
     </row>
@@ -1689,11 +1689,11 @@
         <v>5078</v>
       </c>
       <c r="C70" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>seagateshare.com</t>
+          <t>ipungpurbaya.net</t>
         </is>
       </c>
     </row>
@@ -1707,11 +1707,11 @@
         <v>5078</v>
       </c>
       <c r="C71" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>www.blogpeople.net</t>
+          <t>gfbemail.bbva-bancomer.com</t>
         </is>
       </c>
     </row>
@@ -1725,11 +1725,11 @@
         <v>5078</v>
       </c>
       <c r="C72" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>dinoyy.xyz</t>
+          <t>site-112800294179.gslb1.sakura.ne.jp</t>
         </is>
       </c>
     </row>
@@ -1743,11 +1743,11 @@
         <v>5078</v>
       </c>
       <c r="C73" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>img.tpttzy.com</t>
+          <t>mountfield-events.persoo.xyz</t>
         </is>
       </c>
     </row>
@@ -1761,11 +1761,11 @@
         <v>5078</v>
       </c>
       <c r="C74" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>forum.pcefans.cz</t>
+          <t>jameda-elements.de</t>
         </is>
       </c>
     </row>
@@ -1779,11 +1779,11 @@
         <v>5078</v>
       </c>
       <c r="C75" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>sso.manpower.gov.om</t>
+          <t>catpitaqmi.net</t>
         </is>
       </c>
     </row>
@@ -1797,11 +1797,11 @@
         <v>5078</v>
       </c>
       <c r="C76" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>api.tinyhoneybee.com</t>
+          <t>takungpao.com.hk</t>
         </is>
       </c>
     </row>
@@ -1815,11 +1815,11 @@
         <v>5078</v>
       </c>
       <c r="C77" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>www.cumonprintedpics.com</t>
+          <t>st-fakesysupgrade.fakevivo.com.cn</t>
         </is>
       </c>
     </row>
@@ -1833,11 +1833,11 @@
         <v>5078</v>
       </c>
       <c r="C78" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>network-host.cf</t>
+          <t>tag.contactatonce.co.uk</t>
         </is>
       </c>
     </row>
@@ -1851,11 +1851,11 @@
         <v>5078</v>
       </c>
       <c r="C79" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>custom31335cd6e175f688.dot.cleanbrowsing.org</t>
+          <t>dinoyy.xyz</t>
         </is>
       </c>
     </row>
@@ -1869,11 +1869,11 @@
         <v>5078</v>
       </c>
       <c r="C80" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>preview.page.link</t>
+          <t>img.tpttzy.com</t>
         </is>
       </c>
     </row>
@@ -1887,11 +1887,11 @@
         <v>5078</v>
       </c>
       <c r="C81" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>cpestatus.seagateshare.com</t>
+          <t>forum.pcefans.cz</t>
         </is>
       </c>
     </row>
@@ -1905,11 +1905,11 @@
         <v>5078</v>
       </c>
       <c r="C82" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>indigolbs.dinoyy.xyz</t>
+          <t>r9t1.com</t>
         </is>
       </c>
     </row>
@@ -1923,11 +1923,11 @@
         <v>5078</v>
       </c>
       <c r="C83" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>escambiak12.edu</t>
+          <t>network-host.cf</t>
         </is>
       </c>
     </row>
@@ -1941,11 +1941,11 @@
         <v>5078</v>
       </c>
       <c r="C84" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>as-2314255.cdn.beampulse.com</t>
+          <t>raisingteenstoday.com</t>
         </is>
       </c>
     </row>
@@ -1959,11 +1959,11 @@
         <v>5078</v>
       </c>
       <c r="C85" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>facebookcb.digitaldevs.co.uk</t>
+          <t>blessifyinfotech.com</t>
         </is>
       </c>
     </row>
@@ -1977,11 +1977,11 @@
         <v>5078</v>
       </c>
       <c r="C86" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>tsapi.storyxpress.co</t>
+          <t>indigolbs.dinoyy.xyz</t>
         </is>
       </c>
     </row>
@@ -1995,11 +1995,11 @@
         <v>5078</v>
       </c>
       <c r="C87" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>60493198aa70ac43b4249ef4.endpoint.csper.io</t>
+          <t>escambiak12.edu</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
         <v>5078</v>
       </c>
       <c r="C88" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2031,11 +2031,11 @@
         <v>5078</v>
       </c>
       <c r="C89" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>static.doubleclick.ne</t>
+          <t>betadome.net</t>
         </is>
       </c>
     </row>
@@ -2049,11 +2049,11 @@
         <v>5078</v>
       </c>
       <c r="C90" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>velocitysitemetrics.com</t>
+          <t>shive-hattery.int</t>
         </is>
       </c>
     </row>
@@ -2067,11 +2067,11 @@
         <v>5078</v>
       </c>
       <c r="C91" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>wifihotspot.hu</t>
+          <t>smartstreet.shopinet.xyz</t>
         </is>
       </c>
     </row>
@@ -2085,11 +2085,11 @@
         <v>5078</v>
       </c>
       <c r="C92" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>shive-hattery.int</t>
+          <t>foan2021.eu</t>
         </is>
       </c>
     </row>
@@ -2103,11 +2103,11 @@
         <v>5078</v>
       </c>
       <c r="C93" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>smartstreet.shopinet.xyz</t>
+          <t>cpestatus.seagateshare.com</t>
         </is>
       </c>
     </row>
@@ -2121,47 +2121,47 @@
         <v>5078</v>
       </c>
       <c r="C94" t="n">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>foan2021.eu</t>
+          <t>60493198aa70ac43b4249ef4.endpoint.csper.io</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>tls_root_cert_validity_len</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>5078</v>
+        <v>1349</v>
       </c>
       <c r="C95" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>ipungpurbaya.net</t>
+          <t>cooooos.com</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>tls_root_cert_validity_len</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>5078</v>
+        <v>1349</v>
       </c>
       <c r="C96" t="n">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>gfbemail.bbva-bancomer.com</t>
+          <t>dajak.vafrike.ru</t>
         </is>
       </c>
     </row>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>cooooos.com</t>
+          <t>ailanibah.com</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>dajak.vafrike.ru</t>
+          <t>onbase.space</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>ailanibah.com</t>
+          <t>torrentsmd.me</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>onbase.space</t>
+          <t>cloudbackup.securepoint.de</t>
         </is>
       </c>
     </row>
@@ -2251,79 +2251,79 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>mp3nhacvui.net</t>
+          <t>call.easy2convert4.me</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>tls_root_cert_validity_len</t>
+          <t>lex_name_len</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>1349</v>
+        <v>24</v>
       </c>
       <c r="C102" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>api-player.globalsun.io</t>
+          <t>www.google.com.fritz.box</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>tls_root_cert_validity_len</t>
+          <t>lex_name_len</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>1349</v>
+        <v>24</v>
       </c>
       <c r="C103" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>call.easy2convert4.me</t>
+          <t>cygnetinfotechmanagedservices.com</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>rdap_ip_longest_v4_prefix_len</t>
+          <t>lex_name_len</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C104" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>matomo.mp3y.download</t>
+          <t>image.faultweb.com</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>lex_name_len</t>
+          <t>tls_total_extension_count</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C105" t="n">
         <v>1</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>cygnetinfotechmanagedservices.com</t>
+          <t>diagnostics.omgservice.com</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>www.dewaxyzvw8787.pw</t>
+          <t>cflare.io</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>baipiao-rss.com</t>
+          <t>value-wolf.org</t>
         </is>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>cflare.io</t>
+          <t>urchintelemetry.com</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>iinmobi.com</t>
+          <t>stun.zmzfile.com</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>mail.wavela.bid</t>
+          <t>www.manpower.gov.om</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>rcmdodo.theirving.net</t>
+          <t>baipiao-rss.com</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>biblehu.com</t>
+          <t>iinmobi.com</t>
         </is>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>stun.zmzfile.com</t>
+          <t>biblehu.com</t>
         </is>
       </c>
     </row>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>www.manpower.gov.om</t>
+          <t>adblock-for-chrome.com</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>matrix.matrixmsg.ml</t>
+          <t>520camera.com</t>
         </is>
       </c>
     </row>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>accounts-account-service-prod.hydra.prod.wwrk.co</t>
+          <t>cdn.mypanel.link</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>520camera.com</t>
+          <t>apps.leadspace.86906.fortiweb-cloud-gcp.net</t>
         </is>
       </c>
     </row>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>cdn.mypanel.link</t>
+          <t>androidevlog.com</t>
         </is>
       </c>
     </row>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>lt.logly.co.jp</t>
+          <t>accounts-account-service-prod.hydra.prod.wwrk.co</t>
         </is>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>stat.speed-app.com</t>
+          <t>lt.logly.co.jp</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>androidevlog.com</t>
+          <t>matrix.matrixmsg.ml</t>
         </is>
       </c>
     </row>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>addresseepaper.com</t>
+          <t>deeponlines.com</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>deeponlines.com</t>
+          <t>stat.speed-app.com</t>
         </is>
       </c>
     </row>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>services.keepersecurity.eu</t>
+          <t>addresseepaper.com</t>
         </is>
       </c>
     </row>
@@ -2715,7 +2715,7 @@
         <v>6</v>
       </c>
       <c r="C127" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -2726,18 +2726,18 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>lex_tld_len</t>
+          <t>dns_dn_level</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C128" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>ibaraki-84764.herokussl.com</t>
+          <t>deliciouscheesesfromfrance.com</t>
         </is>
       </c>
     </row>
@@ -2748,14 +2748,14 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C129" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>deliciouscheesesfromfrance.com</t>
+          <t>truefitness.int</t>
         </is>
       </c>
     </row>
@@ -2766,14 +2766,14 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C130" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>www.tapechat.net</t>
+          <t>api.video.browser.tvall.cn</t>
         </is>
       </c>
     </row>
@@ -2784,14 +2784,14 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C131" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>api.zcoup.com</t>
+          <t>www.tapechat.net</t>
         </is>
       </c>
     </row>
@@ -2802,14 +2802,14 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C132" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>static.amp.services</t>
+          <t>api.zcoup.com</t>
         </is>
       </c>
     </row>
@@ -2820,14 +2820,14 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C133" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>wmkankan.com</t>
+          <t>static.amp.services</t>
         </is>
       </c>
     </row>
@@ -2838,10 +2838,10 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C134" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -2856,14 +2856,14 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C135" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>raisingteenstoday.com</t>
+          <t>www.blogpeople.net</t>
         </is>
       </c>
     </row>
@@ -2874,10 +2874,10 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C136" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -2892,10 +2892,10 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C137" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -2910,86 +2910,86 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C138" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>nypd520.com</t>
+          <t>legitville.com</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>dns_dn_level</t>
+          <t>lex_sub_digit_ratio</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>2</v>
+        <v>0.67</v>
       </c>
       <c r="C139" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>legitville.com</t>
+          <t>up.surfsharking.com</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>dns_dn_level</t>
+          <t>dns_zone_entropy</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>2</v>
+        <v>0.53</v>
       </c>
       <c r="C140" t="n">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>synapse.caterpillarcheesecake.xyz</t>
+          <t>matomo.mp3y.download</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>ip_as_address_entropy</t>
+          <t>dns_zone_entropy</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>2</v>
+        <v>0.53</v>
       </c>
       <c r="C141" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>theirving.net</t>
+          <t>video.browser.tvall.cn</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>lex_sub_digit_ratio</t>
+          <t>dns_zone_entropy</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.67</v>
+        <v>0.53</v>
       </c>
       <c r="C142" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>up.surfsharking.com</t>
+          <t>tick.mhpcc.edu</t>
         </is>
       </c>
     </row>
@@ -3003,11 +3003,11 @@
         <v>0.53</v>
       </c>
       <c r="C143" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>a.antlauncher.com</t>
+          <t>farehitchlower.icu</t>
         </is>
       </c>
     </row>
@@ -3021,11 +3021,11 @@
         <v>0.53</v>
       </c>
       <c r="C144" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>tick.mhpcc.edu</t>
+          <t>rock.fotapro.com</t>
         </is>
       </c>
     </row>
@@ -3039,11 +3039,11 @@
         <v>0.53</v>
       </c>
       <c r="C145" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>farehitchlower.icu</t>
+          <t>hkoptimize.com</t>
         </is>
       </c>
     </row>
@@ -3057,47 +3057,47 @@
         <v>0.53</v>
       </c>
       <c r="C146" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>rock.fotapro.com</t>
+          <t>mk-beta.ru</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0.53</v>
+        <v>0</v>
       </c>
       <c r="C147" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>mk-beta.ru</t>
+          <t>mail.wavela.bid</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0.53</v>
+        <v>0</v>
       </c>
       <c r="C148" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>hkoptimize.com</t>
+          <t>tcs-japan.co.jp</t>
         </is>
       </c>
     </row>
@@ -3111,11 +3111,11 @@
         <v>0</v>
       </c>
       <c r="C149" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>skyworthdigital.sjxrbj.com</t>
+          <t>tracker.sylphix.com</t>
         </is>
       </c>
     </row>
@@ -3129,11 +3129,11 @@
         <v>0</v>
       </c>
       <c r="C150" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>tracker.sylphix.com</t>
+          <t>p1prod.cardinalsupportconnect.com</t>
         </is>
       </c>
     </row>
@@ -3147,11 +3147,11 @@
         <v>0</v>
       </c>
       <c r="C151" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>o80433.ingest.sentry.io</t>
+          <t>www.adtaginformer.com</t>
         </is>
       </c>
     </row>
@@ -3165,11 +3165,11 @@
         <v>0</v>
       </c>
       <c r="C152" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>p1prod.cardinalsupportconnect.com</t>
+          <t>www.vysocinaconvention.cz</t>
         </is>
       </c>
     </row>
@@ -3183,11 +3183,11 @@
         <v>0</v>
       </c>
       <c r="C153" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>du.padubicklykraj.cz</t>
+          <t>nasscom-live.com</t>
         </is>
       </c>
     </row>
@@ -3201,299 +3201,351 @@
         <v>0</v>
       </c>
       <c r="C154" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>www.adtaginformer.com</t>
+          <t>tracker.fastdownload.xyz</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
+          <t>rdap_registrant_name_hash</t>
         </is>
       </c>
       <c r="B155" t="n">
         <v>0</v>
       </c>
       <c r="C155" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>johnrosen1.com</t>
+          <t>www.loyalbooks.com</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
+          <t>rdap_registrant_name_hash</t>
         </is>
       </c>
       <c r="B156" t="n">
         <v>0</v>
       </c>
       <c r="C156" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>www.vysocinaconvention.cz</t>
+          <t>yggnode.cf</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
-        </is>
-      </c>
-      <c r="B157" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr"/>
       <c r="C157" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>rentreediscount.com</t>
+          <t>ibaraki-84764.herokussl.com</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
-        </is>
-      </c>
-      <c r="B158" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr"/>
       <c r="C158" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>nasscom-live.com</t>
+          <t>os-api.test.os.qkcorp.net</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
-        </is>
-      </c>
-      <c r="B159" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr"/>
       <c r="C159" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>tracker.fastdownload.xyz</t>
+          <t>awrcaverybrstuktdybstr.com</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
-        </is>
-      </c>
-      <c r="B160" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr"/>
       <c r="C160" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>mailstream-central.mxrecord.mx</t>
+          <t>theirving.net</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
-        </is>
-      </c>
-      <c r="B161" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr"/>
       <c r="C161" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>rplnd5.com</t>
+          <t>download.2.100000003.aovrugcloud.iegcom.com</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
-        </is>
-      </c>
-      <c r="B162" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr"/>
       <c r="C162" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>nutrien-iksmedia-ccm.net</t>
+          <t>laryngectomy.cultivateward.eu</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
-        </is>
-      </c>
-      <c r="B163" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr"/>
       <c r="C163" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>www.loyalbooks.com</t>
+          <t>nutrien-iksmedia-ccm.net</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
-        </is>
-      </c>
-      <c r="B164" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr"/>
       <c r="C164" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>diagnostics.omgservice.com</t>
+          <t>microgalon.com</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
-        </is>
-      </c>
-      <c r="B165" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr"/>
       <c r="C165" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>yggnode.cf</t>
+          <t>saude.abril.com.br</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
-        </is>
-      </c>
-      <c r="B166" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr"/>
       <c r="C166" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>checkmytrip.app.link</t>
+          <t>a.antlauncher.com</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
-        </is>
-      </c>
-      <c r="B167" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr"/>
       <c r="C167" t="n">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>natureapi.com</t>
+          <t>amazonbrowserapp.de</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
-        </is>
-      </c>
-      <c r="B168" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr"/>
       <c r="C168" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>bihamcurchef.cam</t>
+          <t>solnicka.sk</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
-        </is>
-      </c>
-      <c r="B169" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr"/>
       <c r="C169" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>www.qqgametimes.com</t>
+          <t>wmkankan.com</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
-        </is>
-      </c>
-      <c r="B170" t="n">
-        <v>0</v>
-      </c>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr"/>
       <c r="C170" t="n">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
+          <t>www.qqgametimes.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="n">
+        <v>19</v>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>checkmytrip.app.link</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr"/>
+      <c r="C172" t="n">
+        <v>19</v>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
           <t>theplace.bz</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr"/>
+      <c r="C173" t="n">
+        <v>19</v>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>gpvjyx.ssptp4.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr"/>
+      <c r="C174" t="n">
+        <v>19</v>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>avt-usa.net</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>rdap_domain_age</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr"/>
+      <c r="C175" t="n">
+        <v>19</v>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>fastred.biz</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
restructure, fixes and better pdfs
</commit_message>
<xml_diff>
--- a/false_positives/summary_df.xlsx
+++ b/false_positives/summary_df.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D175"/>
+  <dimension ref="A1:D170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,72 +458,72 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>rdap_domain_age</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>8.931168e+17</v>
+        <v>9.04408292e+17</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>yeeterracing.com</t>
+          <t>bannerlord-service-discovery.bannerlord-services-2.net</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>rdap_domain_age</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>8.931168e+17</v>
+        <v>9.04408292e+17</v>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>ticks2.bugsense.com</t>
+          <t>yeeterracing.com</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>rdap_domain_age</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>8.931168e+17</v>
+        <v>9.04408292e+17</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>www.zhcsm.cn</t>
+          <t>video.browser.tvall.cn</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>rdap_domain_active_time</t>
+          <t>rdap_domain_age</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>8.931168e+17</v>
+        <v>9.04408292e+17</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>edoardocolombo.eu</t>
+          <t>gpvjyx.ssptp4.com</t>
         </is>
       </c>
     </row>
@@ -534,14 +534,14 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>8.931168e+17</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>synapse.caterpillarcheesecake.xyz</t>
+          <t>www.zhcsm.cn</t>
         </is>
       </c>
     </row>
@@ -552,140 +552,140 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>8.931168e+17</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C7" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>www.studiumarteterapie.cz</t>
+          <t>babbage.betadome.net</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>rdap_registrar_name_hash</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1757849580</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C8" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>bihamcurchef.cam</t>
+          <t>solnicka.sk</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>5078</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C9" t="n">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>torrentsnows.com</t>
+          <t>intouchservices.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5078</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C10" t="n">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>connect.proxytx.cloud</t>
+          <t>edoardocolombo.eu</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5078</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C11" t="n">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>torrentz2.eu</t>
+          <t>avt-usa.net</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_domain_active_time</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5078</v>
+        <v>7.2576e+17</v>
       </c>
       <c r="C12" t="n">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>sensagent.leparisien.fr</t>
+          <t>www.studiumarteterapie.cz</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_time_from_last_change</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>5078</v>
+        <v>4.00056294e+17</v>
       </c>
       <c r="C13" t="n">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>airportus.info</t>
+          <t>torrentsmd.me</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>tls_root_cert_lifetime</t>
+          <t>rdap_time_from_last_change</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>5078</v>
+        <v>4.00056294e+17</v>
       </c>
       <c r="C14" t="n">
-        <v>86</v>
+        <v>2</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>time.alcanet.no</t>
+          <t>toubiz.de</t>
         </is>
       </c>
     </row>
@@ -699,11 +699,11 @@
         <v>5078</v>
       </c>
       <c r="C15" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>backupaccount.com</t>
+          <t>sso.kkarau.edu.my</t>
         </is>
       </c>
     </row>
@@ -717,11 +717,11 @@
         <v>5078</v>
       </c>
       <c r="C16" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>pthikitpet.com</t>
+          <t>smaxdn.com</t>
         </is>
       </c>
     </row>
@@ -735,11 +735,11 @@
         <v>5078</v>
       </c>
       <c r="C17" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>one.exness.link</t>
+          <t>doogh.club</t>
         </is>
       </c>
     </row>
@@ -753,11 +753,11 @@
         <v>5078</v>
       </c>
       <c r="C18" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>api.wmkankan.com</t>
+          <t>torrentz2.eu</t>
         </is>
       </c>
     </row>
@@ -771,11 +771,11 @@
         <v>5078</v>
       </c>
       <c r="C19" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>awecerybtuitbyatr.com</t>
+          <t>blibli.gw-dv.net</t>
         </is>
       </c>
     </row>
@@ -789,11 +789,11 @@
         <v>5078</v>
       </c>
       <c r="C20" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>gm2.iinmobi.com</t>
+          <t>torrent-download.to</t>
         </is>
       </c>
     </row>
@@ -807,11 +807,11 @@
         <v>5078</v>
       </c>
       <c r="C21" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>airasia.gw-dv.net</t>
+          <t>games4.qqgametimes.com</t>
         </is>
       </c>
     </row>
@@ -825,11 +825,11 @@
         <v>5078</v>
       </c>
       <c r="C22" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>stra.hasmobi.net</t>
+          <t>torrentsnows.com</t>
         </is>
       </c>
     </row>
@@ -843,11 +843,11 @@
         <v>5078</v>
       </c>
       <c r="C23" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>s.ktxtr.com</t>
+          <t>intensive.int</t>
         </is>
       </c>
     </row>
@@ -861,11 +861,11 @@
         <v>5078</v>
       </c>
       <c r="C24" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>www.dontgobaconmyheart.co.uk</t>
+          <t>auth.merrillcorp.com</t>
         </is>
       </c>
     </row>
@@ -879,11 +879,11 @@
         <v>5078</v>
       </c>
       <c r="C25" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>www.estrenospapaya.com</t>
+          <t>chishir.com</t>
         </is>
       </c>
     </row>
@@ -897,11 +897,11 @@
         <v>5078</v>
       </c>
       <c r="C26" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>eservices.manpower.gov.om</t>
+          <t>audiotel.com.mx</t>
         </is>
       </c>
     </row>
@@ -915,11 +915,11 @@
         <v>5078</v>
       </c>
       <c r="C27" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>www.laboratore-proti-koronaviru.cz</t>
+          <t>szhxws.com</t>
         </is>
       </c>
     </row>
@@ -933,11 +933,11 @@
         <v>5078</v>
       </c>
       <c r="C28" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>smaxdn.com</t>
+          <t>airportus.info</t>
         </is>
       </c>
     </row>
@@ -951,11 +951,11 @@
         <v>5078</v>
       </c>
       <c r="C29" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>doogh.club</t>
+          <t>onlineworkplace24.de</t>
         </is>
       </c>
     </row>
@@ -969,11 +969,11 @@
         <v>5078</v>
       </c>
       <c r="C30" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>blibli.gw-dv.net</t>
+          <t>time.alcanet.no</t>
         </is>
       </c>
     </row>
@@ -987,11 +987,11 @@
         <v>5078</v>
       </c>
       <c r="C31" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>torrent-download.to</t>
+          <t>leavehomesafe.gov.hk</t>
         </is>
       </c>
     </row>
@@ -1005,11 +1005,11 @@
         <v>5078</v>
       </c>
       <c r="C32" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>vid-play.com</t>
+          <t>r.blok.link</t>
         </is>
       </c>
     </row>
@@ -1023,11 +1023,11 @@
         <v>5078</v>
       </c>
       <c r="C33" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>intensive.int</t>
+          <t>ppp.xxpwgxx.com</t>
         </is>
       </c>
     </row>
@@ -1041,11 +1041,11 @@
         <v>5078</v>
       </c>
       <c r="C34" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>chishir.com</t>
+          <t>api.video.browser.tvall.cn</t>
         </is>
       </c>
     </row>
@@ -1059,11 +1059,11 @@
         <v>5078</v>
       </c>
       <c r="C35" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>szhxws.com</t>
+          <t>connect.dewvpn.cc</t>
         </is>
       </c>
     </row>
@@ -1077,11 +1077,11 @@
         <v>5078</v>
       </c>
       <c r="C36" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>duckduckmooseapps.com</t>
+          <t>discordapp.page.link</t>
         </is>
       </c>
     </row>
@@ -1095,11 +1095,11 @@
         <v>5078</v>
       </c>
       <c r="C37" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>www.1ucn.com</t>
+          <t>endpointdns-gcprod-use1-lb.jfrog.io</t>
         </is>
       </c>
     </row>
@@ -1113,11 +1113,11 @@
         <v>5078</v>
       </c>
       <c r="C38" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>leavehomesafe.gov.hk</t>
+          <t>pthikitpet.com</t>
         </is>
       </c>
     </row>
@@ -1131,11 +1131,11 @@
         <v>5078</v>
       </c>
       <c r="C39" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>r.blok.link</t>
+          <t>one.exness.link</t>
         </is>
       </c>
     </row>
@@ -1149,11 +1149,11 @@
         <v>5078</v>
       </c>
       <c r="C40" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>tvtelemetrie.de</t>
+          <t>www.centrumprenatalnidiagnostiky.cz</t>
         </is>
       </c>
     </row>
@@ -1167,11 +1167,11 @@
         <v>5078</v>
       </c>
       <c r="C41" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>connect.dewvpn.cc</t>
+          <t>vafrike.ru</t>
         </is>
       </c>
     </row>
@@ -1185,11 +1185,11 @@
         <v>5078</v>
       </c>
       <c r="C42" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>discordapp.page.link</t>
+          <t>www.lnwpickpack.com</t>
         </is>
       </c>
     </row>
@@ -1203,11 +1203,11 @@
         <v>5078</v>
       </c>
       <c r="C43" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>rcmdodo.theirving.net</t>
+          <t>www.yandex.ua</t>
         </is>
       </c>
     </row>
@@ -1221,11 +1221,11 @@
         <v>5078</v>
       </c>
       <c r="C44" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>www.centrumprenatalnidiagnostiky.cz</t>
+          <t>api.wmkankan.com</t>
         </is>
       </c>
     </row>
@@ -1239,11 +1239,11 @@
         <v>5078</v>
       </c>
       <c r="C45" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>vafrike.ru</t>
+          <t>awrcaverybrstuktdybstr.com</t>
         </is>
       </c>
     </row>
@@ -1257,11 +1257,11 @@
         <v>5078</v>
       </c>
       <c r="C46" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>ucmetrixa.info</t>
+          <t>awecerybtuitbyatr.com</t>
         </is>
       </c>
     </row>
@@ -1275,11 +1275,11 @@
         <v>5078</v>
       </c>
       <c r="C47" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>www.mz.de</t>
+          <t>gm2.iinmobi.com</t>
         </is>
       </c>
     </row>
@@ -1293,11 +1293,11 @@
         <v>5078</v>
       </c>
       <c r="C48" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>download.lenovoemc.com</t>
+          <t>airasia.gw-dv.net</t>
         </is>
       </c>
     </row>
@@ -1311,11 +1311,11 @@
         <v>5078</v>
       </c>
       <c r="C49" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>rtbonecode.com</t>
+          <t>tcs-japan.co.jp</t>
         </is>
       </c>
     </row>
@@ -1329,11 +1329,11 @@
         <v>5078</v>
       </c>
       <c r="C50" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>time.nimatronicc.xyz</t>
+          <t>stra.hasmobi.net</t>
         </is>
       </c>
     </row>
@@ -1347,11 +1347,11 @@
         <v>5078</v>
       </c>
       <c r="C51" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>cdn.bitrix24.ua</t>
+          <t>speed-app.com</t>
         </is>
       </c>
     </row>
@@ -1365,11 +1365,11 @@
         <v>5078</v>
       </c>
       <c r="C52" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>bankinformation.1c.ru</t>
+          <t>s.ktxtr.com</t>
         </is>
       </c>
     </row>
@@ -1383,11 +1383,11 @@
         <v>5078</v>
       </c>
       <c r="C53" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>laocaifengxitong.cc</t>
+          <t>download.lenovoemc.com</t>
         </is>
       </c>
     </row>
@@ -1401,11 +1401,11 @@
         <v>5078</v>
       </c>
       <c r="C54" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>ffe390afd658c19dcbf707e0597b846d.de.whecloud.com</t>
+          <t>rtbonecode.com</t>
         </is>
       </c>
     </row>
@@ -1419,11 +1419,11 @@
         <v>5078</v>
       </c>
       <c r="C55" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>update.chupdatebrowserhosting.com</t>
+          <t>insoc.cloud</t>
         </is>
       </c>
     </row>
@@ -1437,11 +1437,11 @@
         <v>5078</v>
       </c>
       <c r="C56" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>ppp.xxpwgxx.com</t>
+          <t>time.nimatronicc.xyz</t>
         </is>
       </c>
     </row>
@@ -1455,11 +1455,11 @@
         <v>5078</v>
       </c>
       <c r="C57" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>sso.manpower.gov.om</t>
+          <t>www.estrenospapaya.com</t>
         </is>
       </c>
     </row>
@@ -1473,11 +1473,11 @@
         <v>5078</v>
       </c>
       <c r="C58" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>www.cumonprintedpics.com</t>
+          <t>eservices.manpower.gov.om</t>
         </is>
       </c>
     </row>
@@ -1491,11 +1491,11 @@
         <v>5078</v>
       </c>
       <c r="C59" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>www.yandex.ua</t>
+          <t>os-api.test.os.qkcorp.net</t>
         </is>
       </c>
     </row>
@@ -1509,11 +1509,11 @@
         <v>5078</v>
       </c>
       <c r="C60" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>vejasp.abril.com.br</t>
+          <t>microgalon.com</t>
         </is>
       </c>
     </row>
@@ -1527,11 +1527,11 @@
         <v>5078</v>
       </c>
       <c r="C61" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>api.tinyhoneybee.com</t>
+          <t>catpitaqmi.net</t>
         </is>
       </c>
     </row>
@@ -1545,11 +1545,11 @@
         <v>5078</v>
       </c>
       <c r="C62" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>services.keepersecurity.eu</t>
+          <t>bankinformation.1c.ru</t>
         </is>
       </c>
     </row>
@@ -1563,11 +1563,11 @@
         <v>5078</v>
       </c>
       <c r="C63" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>www.shorturl.at</t>
+          <t>laocaifengxitong.cc</t>
         </is>
       </c>
     </row>
@@ -1581,11 +1581,11 @@
         <v>5078</v>
       </c>
       <c r="C64" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>transversalnavigation.gamu.cz</t>
+          <t>24.winprizes524.digital</t>
         </is>
       </c>
     </row>
@@ -1599,11 +1599,11 @@
         <v>5078</v>
       </c>
       <c r="C65" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>speed-app.com</t>
+          <t>update.chupdatebrowserhosting.com</t>
         </is>
       </c>
     </row>
@@ -1617,11 +1617,11 @@
         <v>5078</v>
       </c>
       <c r="C66" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>mp3nhacvui.net</t>
+          <t>takungpao.com.hk</t>
         </is>
       </c>
     </row>
@@ -1635,11 +1635,11 @@
         <v>5078</v>
       </c>
       <c r="C67" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>wifihotspot.hu</t>
+          <t>makeawesomeapps.com</t>
         </is>
       </c>
     </row>
@@ -1653,11 +1653,11 @@
         <v>5078</v>
       </c>
       <c r="C68" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>epiccareeverywhere.addenbrookes.nhs.uk</t>
+          <t>st-fakesysupgrade.fakevivo.com.cn</t>
         </is>
       </c>
     </row>
@@ -1671,11 +1671,11 @@
         <v>5078</v>
       </c>
       <c r="C69" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>imagodd.com</t>
+          <t>tag.contactatonce.co.uk</t>
         </is>
       </c>
     </row>
@@ -1689,11 +1689,11 @@
         <v>5078</v>
       </c>
       <c r="C70" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>ipungpurbaya.net</t>
+          <t>seagateshare.com</t>
         </is>
       </c>
     </row>
@@ -1707,11 +1707,11 @@
         <v>5078</v>
       </c>
       <c r="C71" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>gfbemail.bbva-bancomer.com</t>
+          <t>www.blogpeople.net</t>
         </is>
       </c>
     </row>
@@ -1725,11 +1725,11 @@
         <v>5078</v>
       </c>
       <c r="C72" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>site-112800294179.gslb1.sakura.ne.jp</t>
+          <t>dinoyy.xyz</t>
         </is>
       </c>
     </row>
@@ -1743,11 +1743,11 @@
         <v>5078</v>
       </c>
       <c r="C73" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>mountfield-events.persoo.xyz</t>
+          <t>img.tpttzy.com</t>
         </is>
       </c>
     </row>
@@ -1761,11 +1761,11 @@
         <v>5078</v>
       </c>
       <c r="C74" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>jameda-elements.de</t>
+          <t>forum.pcefans.cz</t>
         </is>
       </c>
     </row>
@@ -1779,11 +1779,11 @@
         <v>5078</v>
       </c>
       <c r="C75" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>catpitaqmi.net</t>
+          <t>sso.manpower.gov.om</t>
         </is>
       </c>
     </row>
@@ -1797,11 +1797,11 @@
         <v>5078</v>
       </c>
       <c r="C76" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>takungpao.com.hk</t>
+          <t>api.tinyhoneybee.com</t>
         </is>
       </c>
     </row>
@@ -1815,11 +1815,11 @@
         <v>5078</v>
       </c>
       <c r="C77" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>st-fakesysupgrade.fakevivo.com.cn</t>
+          <t>www.cumonprintedpics.com</t>
         </is>
       </c>
     </row>
@@ -1833,11 +1833,11 @@
         <v>5078</v>
       </c>
       <c r="C78" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>tag.contactatonce.co.uk</t>
+          <t>network-host.cf</t>
         </is>
       </c>
     </row>
@@ -1851,11 +1851,11 @@
         <v>5078</v>
       </c>
       <c r="C79" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>dinoyy.xyz</t>
+          <t>custom31335cd6e175f688.dot.cleanbrowsing.org</t>
         </is>
       </c>
     </row>
@@ -1869,11 +1869,11 @@
         <v>5078</v>
       </c>
       <c r="C80" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>img.tpttzy.com</t>
+          <t>preview.page.link</t>
         </is>
       </c>
     </row>
@@ -1887,11 +1887,11 @@
         <v>5078</v>
       </c>
       <c r="C81" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>forum.pcefans.cz</t>
+          <t>cpestatus.seagateshare.com</t>
         </is>
       </c>
     </row>
@@ -1905,11 +1905,11 @@
         <v>5078</v>
       </c>
       <c r="C82" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>r9t1.com</t>
+          <t>indigolbs.dinoyy.xyz</t>
         </is>
       </c>
     </row>
@@ -1923,11 +1923,11 @@
         <v>5078</v>
       </c>
       <c r="C83" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>network-host.cf</t>
+          <t>escambiak12.edu</t>
         </is>
       </c>
     </row>
@@ -1941,11 +1941,11 @@
         <v>5078</v>
       </c>
       <c r="C84" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>raisingteenstoday.com</t>
+          <t>as-2314255.cdn.beampulse.com</t>
         </is>
       </c>
     </row>
@@ -1959,11 +1959,11 @@
         <v>5078</v>
       </c>
       <c r="C85" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>blessifyinfotech.com</t>
+          <t>facebookcb.digitaldevs.co.uk</t>
         </is>
       </c>
     </row>
@@ -1977,11 +1977,11 @@
         <v>5078</v>
       </c>
       <c r="C86" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>indigolbs.dinoyy.xyz</t>
+          <t>tsapi.storyxpress.co</t>
         </is>
       </c>
     </row>
@@ -1995,11 +1995,11 @@
         <v>5078</v>
       </c>
       <c r="C87" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>escambiak12.edu</t>
+          <t>60493198aa70ac43b4249ef4.endpoint.csper.io</t>
         </is>
       </c>
     </row>
@@ -2013,7 +2013,7 @@
         <v>5078</v>
       </c>
       <c r="C88" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2031,11 +2031,11 @@
         <v>5078</v>
       </c>
       <c r="C89" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>betadome.net</t>
+          <t>static.doubleclick.ne</t>
         </is>
       </c>
     </row>
@@ -2049,11 +2049,11 @@
         <v>5078</v>
       </c>
       <c r="C90" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>shive-hattery.int</t>
+          <t>velocitysitemetrics.com</t>
         </is>
       </c>
     </row>
@@ -2067,11 +2067,11 @@
         <v>5078</v>
       </c>
       <c r="C91" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>smartstreet.shopinet.xyz</t>
+          <t>wifihotspot.hu</t>
         </is>
       </c>
     </row>
@@ -2085,11 +2085,11 @@
         <v>5078</v>
       </c>
       <c r="C92" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>foan2021.eu</t>
+          <t>shive-hattery.int</t>
         </is>
       </c>
     </row>
@@ -2103,11 +2103,11 @@
         <v>5078</v>
       </c>
       <c r="C93" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>cpestatus.seagateshare.com</t>
+          <t>smartstreet.shopinet.xyz</t>
         </is>
       </c>
     </row>
@@ -2121,47 +2121,47 @@
         <v>5078</v>
       </c>
       <c r="C94" t="n">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>60493198aa70ac43b4249ef4.endpoint.csper.io</t>
+          <t>foan2021.eu</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>tls_root_cert_validity_len</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>1349</v>
+        <v>5078</v>
       </c>
       <c r="C95" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>cooooos.com</t>
+          <t>ipungpurbaya.net</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>tls_root_cert_validity_len</t>
+          <t>tls_root_cert_lifetime</t>
         </is>
       </c>
       <c r="B96" t="n">
-        <v>1349</v>
+        <v>5078</v>
       </c>
       <c r="C96" t="n">
-        <v>7</v>
+        <v>82</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>dajak.vafrike.ru</t>
+          <t>gfbemail.bbva-bancomer.com</t>
         </is>
       </c>
     </row>
@@ -2179,7 +2179,7 @@
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>ailanibah.com</t>
+          <t>cooooos.com</t>
         </is>
       </c>
     </row>
@@ -2197,7 +2197,7 @@
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>onbase.space</t>
+          <t>dajak.vafrike.ru</t>
         </is>
       </c>
     </row>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>torrentsmd.me</t>
+          <t>ailanibah.com</t>
         </is>
       </c>
     </row>
@@ -2233,7 +2233,7 @@
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>cloudbackup.securepoint.de</t>
+          <t>onbase.space</t>
         </is>
       </c>
     </row>
@@ -2251,79 +2251,79 @@
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>call.easy2convert4.me</t>
+          <t>mp3nhacvui.net</t>
         </is>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>lex_name_len</t>
+          <t>tls_root_cert_validity_len</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>24</v>
+        <v>1349</v>
       </c>
       <c r="C102" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>www.google.com.fritz.box</t>
+          <t>api-player.globalsun.io</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>lex_name_len</t>
+          <t>tls_root_cert_validity_len</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>24</v>
+        <v>1349</v>
       </c>
       <c r="C103" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>cygnetinfotechmanagedservices.com</t>
+          <t>call.easy2convert4.me</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>lex_name_len</t>
+          <t>rdap_ip_longest_v4_prefix_len</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C104" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>image.faultweb.com</t>
+          <t>matomo.mp3y.download</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>tls_total_extension_count</t>
+          <t>lex_name_len</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C105" t="n">
         <v>1</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>diagnostics.omgservice.com</t>
+          <t>cygnetinfotechmanagedservices.com</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>cflare.io</t>
+          <t>www.dewaxyzvw8787.pw</t>
         </is>
       </c>
     </row>
@@ -2359,7 +2359,7 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>value-wolf.org</t>
+          <t>baipiao-rss.com</t>
         </is>
       </c>
     </row>
@@ -2377,7 +2377,7 @@
       </c>
       <c r="D108" t="inlineStr">
         <is>
-          <t>urchintelemetry.com</t>
+          <t>cflare.io</t>
         </is>
       </c>
     </row>
@@ -2395,7 +2395,7 @@
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>stun.zmzfile.com</t>
+          <t>iinmobi.com</t>
         </is>
       </c>
     </row>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>www.manpower.gov.om</t>
+          <t>mail.wavela.bid</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>baipiao-rss.com</t>
+          <t>rcmdodo.theirving.net</t>
         </is>
       </c>
     </row>
@@ -2449,7 +2449,7 @@
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>iinmobi.com</t>
+          <t>biblehu.com</t>
         </is>
       </c>
     </row>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>biblehu.com</t>
+          <t>stun.zmzfile.com</t>
         </is>
       </c>
     </row>
@@ -2485,7 +2485,7 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>adblock-for-chrome.com</t>
+          <t>www.manpower.gov.om</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>520camera.com</t>
+          <t>matrix.matrixmsg.ml</t>
         </is>
       </c>
     </row>
@@ -2539,7 +2539,7 @@
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>cdn.mypanel.link</t>
+          <t>accounts-account-service-prod.hydra.prod.wwrk.co</t>
         </is>
       </c>
     </row>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>apps.leadspace.86906.fortiweb-cloud-gcp.net</t>
+          <t>520camera.com</t>
         </is>
       </c>
     </row>
@@ -2575,7 +2575,7 @@
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>androidevlog.com</t>
+          <t>cdn.mypanel.link</t>
         </is>
       </c>
     </row>
@@ -2593,7 +2593,7 @@
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>accounts-account-service-prod.hydra.prod.wwrk.co</t>
+          <t>lt.logly.co.jp</t>
         </is>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>lt.logly.co.jp</t>
+          <t>stat.speed-app.com</t>
         </is>
       </c>
     </row>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>matrix.matrixmsg.ml</t>
+          <t>androidevlog.com</t>
         </is>
       </c>
     </row>
@@ -2665,7 +2665,7 @@
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>deeponlines.com</t>
+          <t>addresseepaper.com</t>
         </is>
       </c>
     </row>
@@ -2683,7 +2683,7 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>stat.speed-app.com</t>
+          <t>deeponlines.com</t>
         </is>
       </c>
     </row>
@@ -2701,7 +2701,7 @@
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>addresseepaper.com</t>
+          <t>services.keepersecurity.eu</t>
         </is>
       </c>
     </row>
@@ -2715,7 +2715,7 @@
         <v>6</v>
       </c>
       <c r="C127" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D127" t="inlineStr">
         <is>
@@ -2726,18 +2726,18 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>dns_dn_level</t>
+          <t>lex_tld_len</t>
         </is>
       </c>
       <c r="B128" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C128" t="n">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>deliciouscheesesfromfrance.com</t>
+          <t>ibaraki-84764.herokussl.com</t>
         </is>
       </c>
     </row>
@@ -2748,14 +2748,14 @@
         </is>
       </c>
       <c r="B129" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C129" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>truefitness.int</t>
+          <t>deliciouscheesesfromfrance.com</t>
         </is>
       </c>
     </row>
@@ -2766,14 +2766,14 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C130" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>api.video.browser.tvall.cn</t>
+          <t>www.tapechat.net</t>
         </is>
       </c>
     </row>
@@ -2784,14 +2784,14 @@
         </is>
       </c>
       <c r="B131" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C131" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>www.tapechat.net</t>
+          <t>api.zcoup.com</t>
         </is>
       </c>
     </row>
@@ -2802,14 +2802,14 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C132" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>api.zcoup.com</t>
+          <t>static.amp.services</t>
         </is>
       </c>
     </row>
@@ -2820,14 +2820,14 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C133" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>static.amp.services</t>
+          <t>wmkankan.com</t>
         </is>
       </c>
     </row>
@@ -2838,10 +2838,10 @@
         </is>
       </c>
       <c r="B134" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C134" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D134" t="inlineStr">
         <is>
@@ -2856,14 +2856,14 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C135" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>www.blogpeople.net</t>
+          <t>raisingteenstoday.com</t>
         </is>
       </c>
     </row>
@@ -2874,10 +2874,10 @@
         </is>
       </c>
       <c r="B136" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C136" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D136" t="inlineStr">
         <is>
@@ -2892,10 +2892,10 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C137" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D137" t="inlineStr">
         <is>
@@ -2910,86 +2910,86 @@
         </is>
       </c>
       <c r="B138" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C138" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>legitville.com</t>
+          <t>nypd520.com</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>lex_sub_digit_ratio</t>
+          <t>dns_dn_level</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>0.67</v>
+        <v>2</v>
       </c>
       <c r="C139" t="n">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>up.surfsharking.com</t>
+          <t>legitville.com</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>dns_dn_level</t>
         </is>
       </c>
       <c r="B140" t="n">
-        <v>0.53</v>
+        <v>2</v>
       </c>
       <c r="C140" t="n">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>matomo.mp3y.download</t>
+          <t>synapse.caterpillarcheesecake.xyz</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>ip_as_address_entropy</t>
         </is>
       </c>
       <c r="B141" t="n">
-        <v>0.53</v>
+        <v>2</v>
       </c>
       <c r="C141" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>video.browser.tvall.cn</t>
+          <t>theirving.net</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>dns_zone_entropy</t>
+          <t>lex_sub_digit_ratio</t>
         </is>
       </c>
       <c r="B142" t="n">
-        <v>0.53</v>
+        <v>0.67</v>
       </c>
       <c r="C142" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>tick.mhpcc.edu</t>
+          <t>up.surfsharking.com</t>
         </is>
       </c>
     </row>
@@ -3003,11 +3003,11 @@
         <v>0.53</v>
       </c>
       <c r="C143" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>farehitchlower.icu</t>
+          <t>a.antlauncher.com</t>
         </is>
       </c>
     </row>
@@ -3021,11 +3021,11 @@
         <v>0.53</v>
       </c>
       <c r="C144" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>rock.fotapro.com</t>
+          <t>tick.mhpcc.edu</t>
         </is>
       </c>
     </row>
@@ -3039,11 +3039,11 @@
         <v>0.53</v>
       </c>
       <c r="C145" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>hkoptimize.com</t>
+          <t>farehitchlower.icu</t>
         </is>
       </c>
     </row>
@@ -3057,47 +3057,47 @@
         <v>0.53</v>
       </c>
       <c r="C146" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>mk-beta.ru</t>
+          <t>rock.fotapro.com</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
+          <t>dns_zone_entropy</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="C147" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>mail.wavela.bid</t>
+          <t>mk-beta.ru</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>dns_ttl_low</t>
+          <t>dns_zone_entropy</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>0</v>
+        <v>0.53</v>
       </c>
       <c r="C148" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>tcs-japan.co.jp</t>
+          <t>hkoptimize.com</t>
         </is>
       </c>
     </row>
@@ -3111,11 +3111,11 @@
         <v>0</v>
       </c>
       <c r="C149" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>tracker.sylphix.com</t>
+          <t>skyworthdigital.sjxrbj.com</t>
         </is>
       </c>
     </row>
@@ -3129,11 +3129,11 @@
         <v>0</v>
       </c>
       <c r="C150" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>p1prod.cardinalsupportconnect.com</t>
+          <t>tracker.sylphix.com</t>
         </is>
       </c>
     </row>
@@ -3147,11 +3147,11 @@
         <v>0</v>
       </c>
       <c r="C151" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>www.adtaginformer.com</t>
+          <t>o80433.ingest.sentry.io</t>
         </is>
       </c>
     </row>
@@ -3165,11 +3165,11 @@
         <v>0</v>
       </c>
       <c r="C152" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>www.vysocinaconvention.cz</t>
+          <t>p1prod.cardinalsupportconnect.com</t>
         </is>
       </c>
     </row>
@@ -3183,11 +3183,11 @@
         <v>0</v>
       </c>
       <c r="C153" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>nasscom-live.com</t>
+          <t>du.padubicklykraj.cz</t>
         </is>
       </c>
     </row>
@@ -3201,351 +3201,299 @@
         <v>0</v>
       </c>
       <c r="C154" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>tracker.fastdownload.xyz</t>
+          <t>www.adtaginformer.com</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B155" t="n">
         <v>0</v>
       </c>
       <c r="C155" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>www.loyalbooks.com</t>
+          <t>johnrosen1.com</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>rdap_registrant_name_hash</t>
+          <t>dns_ttl_low</t>
         </is>
       </c>
       <c r="B156" t="n">
         <v>0</v>
       </c>
       <c r="C156" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>yggnode.cf</t>
+          <t>www.vysocinaconvention.cz</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B157" t="inlineStr"/>
+          <t>dns_ttl_low</t>
+        </is>
+      </c>
+      <c r="B157" t="n">
+        <v>0</v>
+      </c>
       <c r="C157" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>ibaraki-84764.herokussl.com</t>
+          <t>rentreediscount.com</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B158" t="inlineStr"/>
+          <t>dns_ttl_low</t>
+        </is>
+      </c>
+      <c r="B158" t="n">
+        <v>0</v>
+      </c>
       <c r="C158" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>os-api.test.os.qkcorp.net</t>
+          <t>nasscom-live.com</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr"/>
+          <t>dns_ttl_low</t>
+        </is>
+      </c>
+      <c r="B159" t="n">
+        <v>0</v>
+      </c>
       <c r="C159" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>awrcaverybrstuktdybstr.com</t>
+          <t>tracker.fastdownload.xyz</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr"/>
+          <t>dns_ttl_low</t>
+        </is>
+      </c>
+      <c r="B160" t="n">
+        <v>0</v>
+      </c>
       <c r="C160" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>theirving.net</t>
+          <t>mailstream-central.mxrecord.mx</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B161" t="inlineStr"/>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B161" t="n">
+        <v>0</v>
+      </c>
       <c r="C161" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>download.2.100000003.aovrugcloud.iegcom.com</t>
+          <t>rplnd5.com</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B162" t="inlineStr"/>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B162" t="n">
+        <v>0</v>
+      </c>
       <c r="C162" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>laryngectomy.cultivateward.eu</t>
+          <t>nutrien-iksmedia-ccm.net</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B163" t="inlineStr"/>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B163" t="n">
+        <v>0</v>
+      </c>
       <c r="C163" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>nutrien-iksmedia-ccm.net</t>
+          <t>www.loyalbooks.com</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B164" t="inlineStr"/>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B164" t="n">
+        <v>0</v>
+      </c>
       <c r="C164" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>microgalon.com</t>
+          <t>diagnostics.omgservice.com</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B165" t="inlineStr"/>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B165" t="n">
+        <v>0</v>
+      </c>
       <c r="C165" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>saude.abril.com.br</t>
+          <t>yggnode.cf</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B166" t="inlineStr"/>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B166" t="n">
+        <v>0</v>
+      </c>
       <c r="C166" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>a.antlauncher.com</t>
+          <t>checkmytrip.app.link</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B167" t="inlineStr"/>
+          <t>rdap_registrant_name_hash</t>
+        </is>
+      </c>
+      <c r="B167" t="n">
+        <v>0</v>
+      </c>
       <c r="C167" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>amazonbrowserapp.de</t>
+          <t>natureapi.com</t>
         </is>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B168" t="inlineStr"/>
+          <t>rdap_registrar_name_hash</t>
+        </is>
+      </c>
+      <c r="B168" t="n">
+        <v>0</v>
+      </c>
       <c r="C168" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>solnicka.sk</t>
+          <t>bihamcurchef.cam</t>
         </is>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr"/>
+          <t>rdap_registrar_name_hash</t>
+        </is>
+      </c>
+      <c r="B169" t="n">
+        <v>0</v>
+      </c>
       <c r="C169" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>wmkankan.com</t>
+          <t>www.qqgametimes.com</t>
         </is>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr"/>
+          <t>rdap_registrar_name_hash</t>
+        </is>
+      </c>
+      <c r="B170" t="n">
+        <v>0</v>
+      </c>
       <c r="C170" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>www.qqgametimes.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="171">
-      <c r="A171" t="inlineStr">
-        <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B171" t="inlineStr"/>
-      <c r="C171" t="n">
-        <v>19</v>
-      </c>
-      <c r="D171" t="inlineStr">
-        <is>
-          <t>checkmytrip.app.link</t>
-        </is>
-      </c>
-    </row>
-    <row r="172">
-      <c r="A172" t="inlineStr">
-        <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B172" t="inlineStr"/>
-      <c r="C172" t="n">
-        <v>19</v>
-      </c>
-      <c r="D172" t="inlineStr">
-        <is>
           <t>theplace.bz</t>
-        </is>
-      </c>
-    </row>
-    <row r="173">
-      <c r="A173" t="inlineStr">
-        <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B173" t="inlineStr"/>
-      <c r="C173" t="n">
-        <v>19</v>
-      </c>
-      <c r="D173" t="inlineStr">
-        <is>
-          <t>gpvjyx.ssptp4.com</t>
-        </is>
-      </c>
-    </row>
-    <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr"/>
-      <c r="C174" t="n">
-        <v>19</v>
-      </c>
-      <c r="D174" t="inlineStr">
-        <is>
-          <t>avt-usa.net</t>
-        </is>
-      </c>
-    </row>
-    <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>rdap_domain_age</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr"/>
-      <c r="C175" t="n">
-        <v>19</v>
-      </c>
-      <c r="D175" t="inlineStr">
-        <is>
-          <t>fastred.biz</t>
         </is>
       </c>
     </row>

</xml_diff>